<commit_message>
FPE - saving of Work In Progress
</commit_message>
<xml_diff>
--- a/FPE/FPE_testpopulatie.xlsx
+++ b/FPE/FPE_testpopulatie.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783DA69F-0144-4863-A6BD-AF938A940408}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2C87A5-3B11-4BB2-9F4E-FB75D2CD5401}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33492" yWindow="-13068" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FLINT Acties" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>actPrecdx</t>
   </si>
@@ -31,12 +31,6 @@
     <t>actPostcdx</t>
   </si>
   <si>
-    <t>actHandeling</t>
-  </si>
-  <si>
-    <t>actRol</t>
-  </si>
-  <si>
     <t>Expressie</t>
   </si>
   <si>
@@ -46,18 +40,9 @@
     <t>Role</t>
   </si>
   <si>
-    <t>[Acties]</t>
-  </si>
-  <si>
-    <t>Actie</t>
-  </si>
-  <si>
     <t>actNaam</t>
   </si>
   <si>
-    <t>ActieNaam</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -122,6 +107,24 @@
   </si>
   <si>
     <t>admin moet klaas op de kandidatenlijst zetten</t>
+  </si>
+  <si>
+    <t>Activiteit</t>
+  </si>
+  <si>
+    <t>[Activiteiten]</t>
+  </si>
+  <si>
+    <t>actRole</t>
+  </si>
+  <si>
+    <t>actRandcdx</t>
+  </si>
+  <si>
+    <t>actVoorschrift</t>
+  </si>
+  <si>
+    <t>ActNaam</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -552,23 +555,23 @@
     <col min="1" max="2" width="17.44140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="29.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="48.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="54.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="80.5546875" style="6" customWidth="1"/>
-    <col min="8" max="10" width="24.77734375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="6" width="48.5546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="80.5546875" style="6" customWidth="1"/>
+    <col min="9" max="11" width="24.77734375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -577,117 +580,123 @@
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="2"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>